<commit_message>
Changed # of TP in configuration files for the correspondence pool test Updated Excel files with test overviews Adapted maxPoolCorrespondences numbers for performing tests
</commit_message>
<xml_diff>
--- a/Test_Overview/Autokalibrierung_Paramtersweep_Werte.xlsx
+++ b/Test_Overview/Autokalibrierung_Paramtersweep_Werte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Keypoint position accuracy</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>0.025-0.2(res 0.025); set to default (0.075) first</t>
+  </si>
+  <si>
+    <t>relMinInlierRatSkip</t>
+  </si>
+  <si>
+    <t>0.4-0.8(0.1res)</t>
   </si>
 </sst>
 </file>
@@ -752,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H36"/>
+  <dimension ref="A2:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +942,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:A36" si="0">A10+1</f>
+        <f t="shared" ref="A11:A37" si="0">A10+1</f>
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1246,11 +1252,15 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>27</v>
+      <c r="B25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25">
+        <f>(0.8-0.4)/0.1+1</f>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1258,108 +1268,105 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>69</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f>(0.8-0.3)/0.1+1</f>
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B27" s="8" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f>(15-1)/2+1</f>
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B28" s="8" t="s">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f>(1000-200)/100+1+(2000-1000)/200+(5000-2000)/500+(10000-5000)/1000+(20000-10000)/2000+(30000-20000)/5000</f>
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-    </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f>(0.2-0.025)/0.025+1</f>
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1368,56 +1375,71 @@
         <v>29</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f>(0.75-0.25)/0.1+1</f>
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f>(0.8-0.1)/0.1+1</f>
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B36" s="8" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <f>(300-20)/20+1</f>
         <v>15</v>
       </c>

</xml_diff>